<commit_message>
hasta categorias de empresa 6 de agosto
</commit_message>
<xml_diff>
--- a/categorias.xlsx
+++ b/categorias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ticom3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AECC6F4A-59E7-40C6-8D66-F41428C07E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7D19C3-E228-4D66-8E17-0BF77BA6CEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{98B6B880-BEA7-4E0F-BB1C-F39BB4B5910B}"/>
+    <workbookView xWindow="4035" yWindow="7005" windowWidth="22590" windowHeight="13305" xr2:uid="{98B6B880-BEA7-4E0F-BB1C-F39BB4B5910B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>